<commit_message>
Latest $VORB balance sheet
</commit_message>
<xml_diff>
--- a/$VORB.xlsx
+++ b/$VORB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB208E9-CC44-4F47-8EF7-FA4CF5A0DEE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12785C6B-10F4-433C-B44A-8A3E350DF994}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{A3F0CF79-FAAB-4BC8-90D6-455BACE41484}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{A3F0CF79-FAAB-4BC8-90D6-455BACE41484}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="145">
   <si>
     <t>$VORB</t>
   </si>
@@ -469,8 +469,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.0\x"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -663,7 +663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -735,40 +735,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="17" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,33 +763,67 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1257,11 +1264,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B74EFA-EB55-4D7D-98D5-0DC814C3F8F0}">
   <dimension ref="B2:AA49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="V34" sqref="V34:AA49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1277,33 +1284,33 @@
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
-      <c r="H5" s="39" t="s">
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="H5" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="41"/>
-      <c r="V5" s="39" t="s">
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="61"/>
+      <c r="V5" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="W5" s="40"/>
-      <c r="X5" s="40"/>
-      <c r="Y5" s="40"/>
-      <c r="Z5" s="40"/>
-      <c r="AA5" s="41"/>
+      <c r="W5" s="60"/>
+      <c r="X5" s="60"/>
+      <c r="Y5" s="60"/>
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="61"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -1325,7 +1332,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="7"/>
-      <c r="V6" s="50" t="s">
+      <c r="V6" s="41" t="s">
         <v>113</v>
       </c>
       <c r="W6" s="6"/>
@@ -1357,7 +1364,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="7"/>
-      <c r="V7" s="56" t="s">
+      <c r="V7" s="47" t="s">
         <v>133</v>
       </c>
       <c r="W7" s="6"/>
@@ -1375,10 +1382,10 @@
         <v>999.5400942199999</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="H8" s="44">
+      <c r="H8" s="35">
         <v>44866</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="36" t="s">
         <v>107</v>
       </c>
       <c r="J8" s="6"/>
@@ -1391,7 +1398,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="7"/>
-      <c r="V8" s="52" t="s">
+      <c r="V8" s="43" t="s">
         <v>134</v>
       </c>
       <c r="W8" s="6"/>
@@ -1404,7 +1411,10 @@
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="15">
+        <f>'Financial Model'!J64</f>
+        <v>71.194000000000003</v>
+      </c>
       <c r="D9" s="17" t="s">
         <v>50</v>
       </c>
@@ -1420,7 +1430,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="7"/>
-      <c r="V9" s="51"/>
+      <c r="V9" s="42"/>
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
@@ -1431,7 +1441,10 @@
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="15">
+        <f>'Financial Model'!J65</f>
+        <v>48.472999999999999</v>
+      </c>
       <c r="D10" s="17" t="s">
         <v>50</v>
       </c>
@@ -1447,7 +1460,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="7"/>
-      <c r="V10" s="56" t="s">
+      <c r="V10" s="47" t="s">
         <v>132</v>
       </c>
       <c r="W10" s="6"/>
@@ -1462,7 +1475,7 @@
       </c>
       <c r="C11" s="15">
         <f>C9-C10</f>
-        <v>0</v>
+        <v>22.721000000000004</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>50</v>
@@ -1479,7 +1492,7 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="7"/>
-      <c r="V11" s="52" t="s">
+      <c r="V11" s="43" t="s">
         <v>135</v>
       </c>
       <c r="W11" s="6"/>
@@ -1494,7 +1507,7 @@
       </c>
       <c r="C12" s="16">
         <f>C8-C11</f>
-        <v>999.5400942199999</v>
+        <v>976.8190942199999</v>
       </c>
       <c r="D12" s="18"/>
       <c r="H12" s="10"/>
@@ -1509,7 +1522,7 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="7"/>
-      <c r="V12" s="53" t="s">
+      <c r="V12" s="44" t="s">
         <v>137</v>
       </c>
       <c r="W12" s="6"/>
@@ -1531,7 +1544,7 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="7"/>
-      <c r="V13" s="51"/>
+      <c r="V13" s="42"/>
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
@@ -1551,7 +1564,7 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="7"/>
-      <c r="V14" s="50" t="s">
+      <c r="V14" s="41" t="s">
         <v>109</v>
       </c>
       <c r="W14" s="6"/>
@@ -1561,11 +1574,11 @@
       <c r="AA14" s="7"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="41"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="61"/>
       <c r="H15" s="10"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -1578,7 +1591,7 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="7"/>
-      <c r="V15" s="56" t="s">
+      <c r="V15" s="47" t="s">
         <v>111</v>
       </c>
       <c r="W15" s="6"/>
@@ -1591,11 +1604,11 @@
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="54" t="s">
+      <c r="D16" s="58"/>
+      <c r="E16" s="45" t="s">
         <v>114</v>
       </c>
       <c r="H16" s="10"/>
@@ -1610,7 +1623,7 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="7"/>
-      <c r="V16" s="53" t="s">
+      <c r="V16" s="44" t="s">
         <v>138</v>
       </c>
       <c r="W16" s="6"/>
@@ -1623,10 +1636,10 @@
       <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="36"/>
+      <c r="D17" s="58"/>
       <c r="H17" s="10"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -1639,7 +1652,7 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="7"/>
-      <c r="V17" s="53" t="s">
+      <c r="V17" s="44" t="s">
         <v>139</v>
       </c>
       <c r="W17" s="6"/>
@@ -1652,8 +1665,8 @@
       <c r="B18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="36"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="58"/>
       <c r="H18" s="10"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -1666,7 +1679,7 @@
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="7"/>
-      <c r="V18" s="53" t="s">
+      <c r="V18" s="44" t="s">
         <v>140</v>
       </c>
       <c r="W18" s="6"/>
@@ -1679,10 +1692,10 @@
       <c r="B19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="38"/>
+      <c r="D19" s="67"/>
       <c r="H19" s="10"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -1695,7 +1708,7 @@
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="7"/>
-      <c r="V19" s="53" t="s">
+      <c r="V19" s="44" t="s">
         <v>141</v>
       </c>
       <c r="W19" s="6"/>
@@ -1717,7 +1730,7 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="7"/>
-      <c r="V20" s="53"/>
+      <c r="V20" s="44"/>
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
@@ -1737,7 +1750,7 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="7"/>
-      <c r="V21" s="56" t="s">
+      <c r="V21" s="47" t="s">
         <v>110</v>
       </c>
       <c r="W21" s="6"/>
@@ -1747,12 +1760,12 @@
       <c r="AA21" s="7"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="41"/>
-      <c r="H22" s="44">
+      <c r="C22" s="60"/>
+      <c r="D22" s="61"/>
+      <c r="H22" s="35">
         <v>44531</v>
       </c>
       <c r="I22" s="6" t="s">
@@ -1768,7 +1781,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="7"/>
-      <c r="V22" s="53" t="s">
+      <c r="V22" s="44" t="s">
         <v>118</v>
       </c>
       <c r="W22" s="6"/>
@@ -1781,12 +1794,12 @@
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="36"/>
+      <c r="D23" s="58"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="60" t="s">
+      <c r="I23" s="49" t="s">
         <v>124</v>
       </c>
       <c r="J23" s="6"/>
@@ -1799,7 +1812,7 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="7"/>
-      <c r="V23" s="49"/>
+      <c r="V23" s="40"/>
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
@@ -1810,10 +1823,10 @@
       <c r="B24" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="35">
+      <c r="C24" s="57">
         <v>2017</v>
       </c>
-      <c r="D24" s="36"/>
+      <c r="D24" s="58"/>
       <c r="H24" s="10"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
@@ -1826,7 +1839,7 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="7"/>
-      <c r="V24" s="56" t="s">
+      <c r="V24" s="47" t="s">
         <v>136</v>
       </c>
       <c r="W24" s="6"/>
@@ -1839,10 +1852,10 @@
       <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="58">
+      <c r="C25" s="62">
         <v>44560</v>
       </c>
-      <c r="D25" s="59"/>
+      <c r="D25" s="63"/>
       <c r="H25" s="10"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
@@ -1855,7 +1868,7 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="7"/>
-      <c r="V25" s="53" t="s">
+      <c r="V25" s="44" t="s">
         <v>119</v>
       </c>
       <c r="W25" s="6"/>
@@ -1866,12 +1879,12 @@
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B26" s="10"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="H26" s="44">
+      <c r="C26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="H26" s="35">
         <v>44501</v>
       </c>
-      <c r="I26" s="45" t="s">
+      <c r="I26" s="36" t="s">
         <v>144</v>
       </c>
       <c r="J26" s="6"/>
@@ -1884,7 +1897,7 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
       <c r="S26" s="7"/>
-      <c r="V26" s="49"/>
+      <c r="V26" s="40"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
       <c r="Y26" s="6"/>
@@ -1893,8 +1906,8 @@
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B27" s="10"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="36"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
       <c r="H27" s="10"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -1907,7 +1920,7 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="7"/>
-      <c r="V27" s="56" t="s">
+      <c r="V27" s="47" t="s">
         <v>112</v>
       </c>
       <c r="W27" s="6"/>
@@ -1938,7 +1951,7 @@
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
       <c r="S28" s="7"/>
-      <c r="V28" s="53" t="s">
+      <c r="V28" s="44" t="s">
         <v>120</v>
       </c>
       <c r="W28" s="6"/>
@@ -1951,10 +1964,10 @@
       <c r="B29" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="43"/>
+      <c r="D29" s="69"/>
       <c r="H29" s="10"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
@@ -1967,7 +1980,7 @@
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
       <c r="S29" s="7"/>
-      <c r="V29" s="57" t="s">
+      <c r="V29" s="48" t="s">
         <v>121</v>
       </c>
       <c r="W29" s="6"/>
@@ -1989,7 +2002,7 @@
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
       <c r="S30" s="7"/>
-      <c r="V30" s="49"/>
+      <c r="V30" s="40"/>
       <c r="W30" s="6"/>
       <c r="X30" s="6"/>
       <c r="Y30" s="6"/>
@@ -2009,7 +2022,7 @@
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
       <c r="S31" s="7"/>
-      <c r="V31" s="56" t="s">
+      <c r="V31" s="47" t="s">
         <v>142</v>
       </c>
       <c r="W31" s="6"/>
@@ -2019,11 +2032,11 @@
       <c r="AA31" s="7"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="41"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="61"/>
       <c r="H32" s="10"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
@@ -2036,7 +2049,7 @@
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
       <c r="S32" s="7"/>
-      <c r="V32" s="53" t="s">
+      <c r="V32" s="44" t="s">
         <v>143</v>
       </c>
       <c r="W32" s="6"/>
@@ -2049,8 +2062,11 @@
       <c r="B33" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="36"/>
+      <c r="C33" s="70">
+        <f>C6/'Financial Model'!J62</f>
+        <v>11.16966815537452</v>
+      </c>
+      <c r="D33" s="71"/>
       <c r="H33" s="10"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
@@ -2063,7 +2079,7 @@
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
       <c r="S33" s="7"/>
-      <c r="V33" s="49"/>
+      <c r="V33" s="40"/>
       <c r="W33" s="6"/>
       <c r="X33" s="6"/>
       <c r="Y33" s="6"/>
@@ -2074,8 +2090,8 @@
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="36"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
       <c r="H34" s="10"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
@@ -2088,7 +2104,7 @@
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
       <c r="S34" s="7"/>
-      <c r="V34" s="50" t="s">
+      <c r="V34" s="41" t="s">
         <v>117</v>
       </c>
       <c r="W34" s="6"/>
@@ -2101,8 +2117,8 @@
       <c r="B35" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="36"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
       <c r="H35" s="10"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
@@ -2115,7 +2131,7 @@
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
       <c r="S35" s="7"/>
-      <c r="V35" s="51" t="s">
+      <c r="V35" s="42" t="s">
         <v>115</v>
       </c>
       <c r="W35" s="6"/>
@@ -2128,8 +2144,8 @@
       <c r="B36" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="37"/>
-      <c r="D36" s="38"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="67"/>
       <c r="H36" s="11"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
@@ -2142,7 +2158,7 @@
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
       <c r="S36" s="9"/>
-      <c r="V36" s="55" t="s">
+      <c r="V36" s="46" t="s">
         <v>116</v>
       </c>
       <c r="W36" s="8"/>
@@ -2152,29 +2168,29 @@
       <c r="AA36" s="9"/>
     </row>
     <row r="39" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="41"/>
-      <c r="V39" s="39" t="s">
+      <c r="C39" s="60"/>
+      <c r="D39" s="61"/>
+      <c r="V39" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="W39" s="40"/>
-      <c r="X39" s="40"/>
-      <c r="Y39" s="40"/>
-      <c r="Z39" s="40"/>
-      <c r="AA39" s="41"/>
+      <c r="W39" s="60"/>
+      <c r="X39" s="60"/>
+      <c r="Y39" s="60"/>
+      <c r="Z39" s="60"/>
+      <c r="AA39" s="61"/>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B40" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="67" t="s">
+      <c r="C40" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="68"/>
-      <c r="V40" s="61"/>
+      <c r="D40" s="65"/>
+      <c r="V40" s="50"/>
       <c r="W40" s="6"/>
       <c r="X40" s="6"/>
       <c r="Y40" s="6"/>
@@ -2185,7 +2201,7 @@
       <c r="B41" s="10"/>
       <c r="C41" s="30"/>
       <c r="D41" s="31"/>
-      <c r="V41" s="61"/>
+      <c r="V41" s="50"/>
       <c r="W41" s="6"/>
       <c r="X41" s="6"/>
       <c r="Y41" s="6"/>
@@ -2196,7 +2212,7 @@
       <c r="B42" s="10"/>
       <c r="C42" s="30"/>
       <c r="D42" s="31"/>
-      <c r="V42" s="62">
+      <c r="V42" s="51">
         <v>44562</v>
       </c>
       <c r="W42" s="6" t="s">
@@ -2211,7 +2227,8 @@
       <c r="B43" s="11"/>
       <c r="C43" s="32"/>
       <c r="D43" s="33"/>
-      <c r="V43" s="61"/>
+      <c r="J43" s="56"/>
+      <c r="V43" s="50"/>
       <c r="W43" s="6"/>
       <c r="X43" s="6"/>
       <c r="Y43" s="6"/>
@@ -2219,7 +2236,7 @@
       <c r="AA43" s="7"/>
     </row>
     <row r="44" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="V44" s="62">
+      <c r="V44" s="51">
         <v>44348</v>
       </c>
       <c r="W44" s="6" t="s">
@@ -2231,7 +2248,7 @@
       <c r="AA44" s="7"/>
     </row>
     <row r="45" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="V45" s="61"/>
+      <c r="V45" s="50"/>
       <c r="W45" s="6"/>
       <c r="X45" s="6"/>
       <c r="Y45" s="6"/>
@@ -2239,7 +2256,7 @@
       <c r="AA45" s="7"/>
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="V46" s="62">
+      <c r="V46" s="51">
         <v>44197</v>
       </c>
       <c r="W46" s="6" t="s">
@@ -2251,8 +2268,8 @@
       <c r="AA46" s="7"/>
     </row>
     <row r="47" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="V47" s="61"/>
-      <c r="W47" s="63" t="s">
+      <c r="V47" s="50"/>
+      <c r="W47" s="52" t="s">
         <v>127</v>
       </c>
       <c r="X47" s="6"/>
@@ -2261,7 +2278,7 @@
       <c r="AA47" s="7"/>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="V48" s="61"/>
+      <c r="V48" s="50"/>
       <c r="W48" s="6"/>
       <c r="X48" s="6"/>
       <c r="Y48" s="6"/>
@@ -2269,16 +2286,16 @@
       <c r="AA48" s="7"/>
     </row>
     <row r="49" spans="22:27" x14ac:dyDescent="0.2">
-      <c r="V49" s="64">
+      <c r="V49" s="53">
         <v>43952</v>
       </c>
       <c r="W49" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="X49" s="65"/>
-      <c r="Y49" s="65"/>
-      <c r="Z49" s="65"/>
-      <c r="AA49" s="66"/>
+      <c r="X49" s="54"/>
+      <c r="Y49" s="54"/>
+      <c r="Z49" s="54"/>
+      <c r="AA49" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -2298,13 +2315,13 @@
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{D9BC7303-6CA5-439B-B622-1349F7C34E60}"/>
@@ -2321,14 +2338,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBA637C-06CC-410C-8E71-3A4C3B33A1DE}">
   <dimension ref="B1:AE75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -2446,7 +2463,7 @@
       <c r="B4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="38">
         <v>1.6930000000000001</v>
       </c>
       <c r="F4" s="27">
@@ -2463,7 +2480,7 @@
       <c r="B5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="37">
         <v>14.292</v>
       </c>
       <c r="F5" s="26">
@@ -2480,7 +2497,7 @@
       <c r="B6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="38">
         <f>E4-E5</f>
         <v>-12.599</v>
       </c>
@@ -2501,7 +2518,7 @@
       <c r="B7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="37">
         <v>20.48</v>
       </c>
       <c r="F7" s="26">
@@ -2518,7 +2535,7 @@
       <c r="B8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="37">
         <v>11.616</v>
       </c>
       <c r="F8" s="26">
@@ -2535,7 +2552,7 @@
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="38">
         <f>E6-E7-E8</f>
         <v>-44.695</v>
       </c>
@@ -2556,7 +2573,7 @@
       <c r="B10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="37">
         <v>0</v>
       </c>
       <c r="F10" s="26">
@@ -2573,7 +2590,7 @@
       <c r="B11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="37">
         <v>0</v>
       </c>
       <c r="F11" s="26">
@@ -2590,7 +2607,7 @@
       <c r="B12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="37">
         <v>0</v>
       </c>
       <c r="F12" s="26">
@@ -2607,7 +2624,7 @@
       <c r="B13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="46">
+      <c r="E13" s="37">
         <v>-6.0000000000000001E-3</v>
       </c>
       <c r="F13" s="26">
@@ -2624,7 +2641,7 @@
       <c r="B14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="37">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F14" s="26">
@@ -2641,7 +2658,7 @@
       <c r="B15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="37">
         <f>SUM(E10:E14)</f>
         <v>4.7E-2</v>
       </c>
@@ -2662,7 +2679,7 @@
       <c r="B16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="46">
+      <c r="E16" s="37">
         <f>E9+E15</f>
         <v>-44.648000000000003</v>
       </c>
@@ -2683,7 +2700,7 @@
       <c r="B17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="46">
+      <c r="E17" s="37">
         <v>0</v>
       </c>
       <c r="F17" s="26">
@@ -2700,7 +2717,7 @@
       <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="47">
+      <c r="E18" s="38">
         <f>E16-E17</f>
         <v>-44.648000000000003</v>
       </c>
@@ -2748,7 +2765,7 @@
       <c r="F20" s="26">
         <v>294.124548</v>
       </c>
-      <c r="I20" s="46">
+      <c r="I20" s="37">
         <v>334.96193199999999</v>
       </c>
       <c r="J20" s="26">
@@ -2759,6 +2776,9 @@
       <c r="B22" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="E22" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="F22" s="14" t="s">
         <v>76</v>
       </c>
@@ -2779,7 +2799,24 @@
       <c r="B23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J23" s="29"/>
+      <c r="E23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
@@ -2858,47 +2895,62 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I33" s="27">
         <v>122.072</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="27">
+        <v>71.194000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>78</v>
       </c>
       <c r="I34" s="26">
         <v>0.82799999999999996</v>
       </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>79</v>
       </c>
       <c r="I35" s="26">
         <v>11.263</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="26">
+        <v>1.9770000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>80</v>
       </c>
       <c r="I36" s="26">
         <v>66.528999999999996</v>
       </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="26">
+        <v>69.228999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>81</v>
       </c>
       <c r="I37" s="26">
         <v>15.122</v>
       </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J37" s="26">
+        <v>12.708</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>82</v>
       </c>
@@ -2906,40 +2958,56 @@
         <f>SUM(I33:I37)</f>
         <v>215.81400000000002</v>
       </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J38" s="26">
+        <f>SUM(J33:J37)</f>
+        <v>155.108</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>83</v>
       </c>
       <c r="I39" s="26">
         <v>65.837999999999994</v>
       </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J39" s="26">
+        <v>69.84</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>84</v>
       </c>
       <c r="I40" s="26">
         <v>12.986000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J40" s="26">
+        <v>13.311999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>85</v>
       </c>
       <c r="I41" s="27">
         <v>4.6779999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J41" s="27">
+        <v>4.3380000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>86</v>
       </c>
       <c r="I42" s="26">
         <v>1.4039999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J42" s="26">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>87</v>
       </c>
@@ -2947,51 +3015,70 @@
         <f>I38+SUM(I39:I42)</f>
         <v>300.72000000000003</v>
       </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J43" s="26">
+        <f>J38+SUM(J39:J42)</f>
+        <v>242.97800000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="I44" s="26"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>88</v>
       </c>
       <c r="I45" s="26">
         <v>9.0640000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J45" s="26">
+        <v>19.728000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>89</v>
       </c>
       <c r="I46" s="26">
         <v>1.3480000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J46" s="26">
+        <v>1.4550000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>90</v>
       </c>
       <c r="I47" s="26">
         <v>4.75</v>
       </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J47" s="26">
+        <v>8.0540000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>91</v>
       </c>
       <c r="I48" s="26">
         <v>22.611000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J48" s="26">
+        <v>25.094000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>92</v>
       </c>
       <c r="I49" s="26">
         <v>37.329000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J49" s="26">
+        <v>17.927</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>93</v>
       </c>
@@ -2999,48 +3086,67 @@
         <f>SUM(I45:I49)</f>
         <v>75.102000000000004</v>
       </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J50" s="26">
+        <f>SUM(J45:J49)</f>
+        <v>72.25800000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I51" s="26">
         <v>12.595000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J51" s="26">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>92</v>
       </c>
       <c r="I52" s="26">
         <v>20.753</v>
       </c>
-    </row>
-    <row r="53" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J52" s="26">
+        <v>9.1649999999999991</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
         <v>95</v>
       </c>
       <c r="I53" s="27">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="2:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J53" s="27">
+        <v>44.146999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
         <v>96</v>
       </c>
       <c r="I54" s="27">
         <v>8.5079999999999991</v>
       </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J54" s="27">
+        <v>4.3259999999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>97</v>
       </c>
       <c r="I55" s="26">
         <v>9.6449999999999996</v>
       </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J55" s="26">
+        <v>10.795</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>98</v>
       </c>
@@ -3048,16 +3154,23 @@
         <f>I50+SUM(I51:I55)</f>
         <v>176.60300000000001</v>
       </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J56" s="26">
+        <f>J50+SUM(J51:J55)</f>
+        <v>153.49099999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>99</v>
       </c>
       <c r="I58" s="26">
         <v>124.117</v>
       </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J58" s="26">
+        <v>89.486999999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>100</v>
       </c>
@@ -3065,8 +3178,12 @@
         <f>I58+I56</f>
         <v>300.72000000000003</v>
       </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J59" s="26">
+        <f>J58+J56</f>
+        <v>242.97799999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>101</v>
       </c>
@@ -3074,8 +3191,12 @@
         <f>I43-I56</f>
         <v>124.11700000000002</v>
       </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J61" s="26">
+        <f t="shared" ref="J61" si="0">J43-J56</f>
+        <v>89.487000000000023</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>102</v>
       </c>
@@ -3083,8 +3204,12 @@
         <f>I61/I20</f>
         <v>0.37054061414955064</v>
       </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="J62" s="1">
+        <f t="shared" ref="J62" si="1">J61/J20</f>
+        <v>0.26679396008431194</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>6</v>
       </c>
@@ -3092,6 +3217,10 @@
         <f>I33</f>
         <v>122.072</v>
       </c>
+      <c r="J64" s="26">
+        <f t="shared" ref="J64" si="2">J33</f>
+        <v>71.194000000000003</v>
+      </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
@@ -3101,6 +3230,10 @@
         <f>I53+I54</f>
         <v>58.507999999999996</v>
       </c>
+      <c r="J65" s="26">
+        <f t="shared" ref="J65" si="3">J53+J54</f>
+        <v>48.472999999999999</v>
+      </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
@@ -3110,6 +3243,10 @@
         <f>I64-I65</f>
         <v>63.564000000000007</v>
       </c>
+      <c r="J66" s="26">
+        <f t="shared" ref="J66" si="4">J64-J65</f>
+        <v>22.721000000000004</v>
+      </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
@@ -3130,6 +3267,10 @@
         <f>I68*I20</f>
         <v>1282.9041995600001</v>
       </c>
+      <c r="J69" s="26">
+        <f t="shared" ref="J69" si="5">J68*J20</f>
+        <v>1029.7275467299999</v>
+      </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
@@ -3139,14 +3280,22 @@
         <f>I69-I66</f>
         <v>1219.34019956</v>
       </c>
+      <c r="J70" s="26">
+        <f t="shared" ref="J70" si="6">J69-J66</f>
+        <v>1007.0065467299999</v>
+      </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="48">
+      <c r="I72" s="39">
         <f>I68/I62</f>
         <v>10.336248858415848</v>
+      </c>
+      <c r="J72" s="39">
+        <f t="shared" ref="J72" si="7">J68/J62</f>
+        <v>11.507007126509992</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.2">
@@ -3170,6 +3319,7 @@
     <hyperlink ref="I1" r:id="rId2" xr:uid="{BB0427F8-D14E-4903-9B79-44B053E9EE3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add aircraft info (reg + tracker link)
</commit_message>
<xml_diff>
--- a/$VORB.xlsx
+++ b/$VORB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12785C6B-10F4-433C-B44A-8A3E350DF994}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D30C40A-D39D-B749-AD8C-557D195545B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{A3F0CF79-FAAB-4BC8-90D6-455BACE41484}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{A3F0CF79-FAAB-4BC8-90D6-455BACE41484}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="148">
   <si>
     <t>$VORB</t>
   </si>
@@ -461,6 +471,15 @@
   </si>
   <si>
     <t>ANA Holdings &amp; Virgin Orbit sign agreement to launch 20 flights of LauncherOne from Oita spaceport in Japan</t>
+  </si>
+  <si>
+    <t>Aircraft</t>
+  </si>
+  <si>
+    <t>N744V</t>
+  </si>
+  <si>
+    <t>B747-4</t>
   </si>
 </sst>
 </file>
@@ -663,7 +682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -784,16 +803,46 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -802,28 +851,10 @@
     <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1262,28 +1293,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B74EFA-EB55-4D7D-98D5-0DC814C3F8F0}">
-  <dimension ref="B2:AA49"/>
+  <dimension ref="B2:AA50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B5" s="59" t="s">
         <v>15</v>
       </c>
@@ -1312,7 +1343,7 @@
       <c r="Z5" s="60"/>
       <c r="AA5" s="61"/>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1341,7 +1372,7 @@
       <c r="Z6" s="6"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1373,7 +1404,7 @@
       <c r="Z7" s="6"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1407,7 +1438,7 @@
       <c r="Z8" s="6"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1437,7 +1468,7 @@
       <c r="Z9" s="6"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1469,7 +1500,7 @@
       <c r="Z10" s="6"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1501,7 +1532,7 @@
       <c r="Z11" s="6"/>
       <c r="AA11" s="7"/>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1531,7 +1562,7 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="7"/>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.15">
       <c r="H13" s="10"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -1551,7 +1582,7 @@
       <c r="Z13" s="6"/>
       <c r="AA13" s="7"/>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.15">
       <c r="H14" s="10"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -1573,7 +1604,7 @@
       <c r="Z14" s="6"/>
       <c r="AA14" s="7"/>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B15" s="59" t="s">
         <v>10</v>
       </c>
@@ -1600,14 +1631,14 @@
       <c r="Z15" s="6"/>
       <c r="AA15" s="7"/>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="58"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="45" t="s">
         <v>114</v>
       </c>
@@ -1632,14 +1663,14 @@
       <c r="Z16" s="6"/>
       <c r="AA16" s="7"/>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="58"/>
+      <c r="D17" s="67"/>
       <c r="H17" s="10"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -1661,12 +1692,12 @@
       <c r="Z17" s="6"/>
       <c r="AA17" s="7"/>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="67"/>
       <c r="H18" s="10"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -1688,14 +1719,14 @@
       <c r="Z18" s="6"/>
       <c r="AA18" s="7"/>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="67"/>
+      <c r="D19" s="65"/>
       <c r="H19" s="10"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -1717,7 +1748,7 @@
       <c r="Z19" s="6"/>
       <c r="AA19" s="7"/>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.15">
       <c r="H20" s="10"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -1737,7 +1768,7 @@
       <c r="Z20" s="6"/>
       <c r="AA20" s="7"/>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.15">
       <c r="H21" s="10"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -1759,7 +1790,7 @@
       <c r="Z21" s="6"/>
       <c r="AA21" s="7"/>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B22" s="59" t="s">
         <v>2</v>
       </c>
@@ -1790,14 +1821,14 @@
       <c r="Z22" s="6"/>
       <c r="AA22" s="7"/>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="58"/>
+      <c r="D23" s="67"/>
       <c r="H23" s="10"/>
       <c r="I23" s="49" t="s">
         <v>124</v>
@@ -1819,14 +1850,14 @@
       <c r="Z23" s="6"/>
       <c r="AA23" s="7"/>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B24" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="57">
+      <c r="C24" s="66">
         <v>2017</v>
       </c>
-      <c r="D24" s="58"/>
+      <c r="D24" s="67"/>
       <c r="H24" s="10"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
@@ -1848,14 +1879,14 @@
       <c r="Z24" s="6"/>
       <c r="AA24" s="7"/>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="72">
         <v>44560</v>
       </c>
-      <c r="D25" s="63"/>
+      <c r="D25" s="73"/>
       <c r="H25" s="10"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
@@ -1877,10 +1908,10 @@
       <c r="Z25" s="6"/>
       <c r="AA25" s="7"/>
     </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B26" s="10"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="67"/>
       <c r="H26" s="35">
         <v>44501</v>
       </c>
@@ -1904,10 +1935,10 @@
       <c r="Z26" s="6"/>
       <c r="AA26" s="7"/>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B27" s="10"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="67"/>
       <c r="H27" s="10"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -1929,7 +1960,7 @@
       <c r="Z27" s="6"/>
       <c r="AA27" s="7"/>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B28" s="10" t="s">
         <v>19</v>
       </c>
@@ -1960,7 +1991,7 @@
       <c r="Z28" s="6"/>
       <c r="AA28" s="7"/>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B29" s="11" t="s">
         <v>20</v>
       </c>
@@ -1989,7 +2020,7 @@
       <c r="Z29" s="6"/>
       <c r="AA29" s="7"/>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.15">
       <c r="H30" s="10"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
@@ -2009,7 +2040,7 @@
       <c r="Z30" s="6"/>
       <c r="AA30" s="7"/>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:27" x14ac:dyDescent="0.15">
       <c r="H31" s="10"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
@@ -2031,7 +2062,7 @@
       <c r="Z31" s="6"/>
       <c r="AA31" s="7"/>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B32" s="59" t="s">
         <v>22</v>
       </c>
@@ -2058,7 +2089,7 @@
       <c r="Z32" s="6"/>
       <c r="AA32" s="7"/>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B33" s="10" t="s">
         <v>23</v>
       </c>
@@ -2086,12 +2117,12 @@
       <c r="Z33" s="6"/>
       <c r="AA33" s="7"/>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="67"/>
       <c r="H34" s="10"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
@@ -2113,12 +2144,12 @@
       <c r="Z34" s="6"/>
       <c r="AA34" s="7"/>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B35" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="58"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="67"/>
       <c r="H35" s="10"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
@@ -2140,12 +2171,12 @@
       <c r="Z35" s="6"/>
       <c r="AA35" s="7"/>
     </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B36" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="66"/>
-      <c r="D36" s="67"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="65"/>
       <c r="H36" s="11"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
@@ -2167,7 +2198,7 @@
       <c r="Z36" s="8"/>
       <c r="AA36" s="9"/>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B39" s="59" t="s">
         <v>131</v>
       </c>
@@ -2182,14 +2213,14 @@
       <c r="Z39" s="60"/>
       <c r="AA39" s="61"/>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B40" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="64" t="s">
+      <c r="C40" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="65"/>
+      <c r="D40" s="63"/>
       <c r="V40" s="50"/>
       <c r="W40" s="6"/>
       <c r="X40" s="6"/>
@@ -2197,7 +2228,7 @@
       <c r="Z40" s="6"/>
       <c r="AA40" s="7"/>
     </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B41" s="10"/>
       <c r="C41" s="30"/>
       <c r="D41" s="31"/>
@@ -2208,7 +2239,7 @@
       <c r="Z41" s="6"/>
       <c r="AA41" s="7"/>
     </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B42" s="10"/>
       <c r="C42" s="30"/>
       <c r="D42" s="31"/>
@@ -2223,7 +2254,7 @@
       <c r="Z42" s="6"/>
       <c r="AA42" s="7"/>
     </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B43" s="11"/>
       <c r="C43" s="32"/>
       <c r="D43" s="33"/>
@@ -2235,7 +2266,7 @@
       <c r="Z43" s="6"/>
       <c r="AA43" s="7"/>
     </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.15">
       <c r="V44" s="51">
         <v>44348</v>
       </c>
@@ -2247,7 +2278,7 @@
       <c r="Z44" s="6"/>
       <c r="AA44" s="7"/>
     </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.15">
       <c r="V45" s="50"/>
       <c r="W45" s="6"/>
       <c r="X45" s="6"/>
@@ -2255,7 +2286,12 @@
       <c r="Z45" s="6"/>
       <c r="AA45" s="7"/>
     </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B46" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="60"/>
+      <c r="D46" s="61"/>
       <c r="V46" s="51">
         <v>44197</v>
       </c>
@@ -2267,7 +2303,14 @@
       <c r="Z46" s="6"/>
       <c r="AA46" s="7"/>
     </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B47" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="7"/>
       <c r="V47" s="50"/>
       <c r="W47" s="52" t="s">
         <v>127</v>
@@ -2277,7 +2320,10 @@
       <c r="Z47" s="6"/>
       <c r="AA47" s="7"/>
     </row>
-    <row r="48" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B48" s="50"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="7"/>
       <c r="V48" s="50"/>
       <c r="W48" s="6"/>
       <c r="X48" s="6"/>
@@ -2285,7 +2331,10 @@
       <c r="Z48" s="6"/>
       <c r="AA48" s="7"/>
     </row>
-    <row r="49" spans="22:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B49" s="50"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="7"/>
       <c r="V49" s="53">
         <v>43952</v>
       </c>
@@ -2297,8 +2346,21 @@
       <c r="Z49" s="54"/>
       <c r="AA49" s="55"/>
     </row>
+    <row r="50" spans="2:27" x14ac:dyDescent="0.15">
+      <c r="B50" s="75"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="V5:AA5"/>
     <mergeCell ref="V39:AA39"/>
     <mergeCell ref="B39:D39"/>
@@ -2315,22 +2377,16 @@
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{D9BC7303-6CA5-439B-B622-1349F7C34E60}"/>
     <hyperlink ref="I8" r:id="rId2" xr:uid="{E39DBCF5-486C-40D8-8DE7-3B1B2093CF5E}"/>
     <hyperlink ref="C40:D40" r:id="rId3" display="Link" xr:uid="{2B0F95BB-3327-4579-B7A8-ECBB8C4B69A6}"/>
     <hyperlink ref="I26" r:id="rId4" xr:uid="{FD0C5381-0521-4F12-85A8-E23C70816062}"/>
+    <hyperlink ref="B47" r:id="rId5" location="flightPageActivityLog" xr:uid="{0D1432A5-D70D-A641-98CE-1CDD0A717403}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2338,21 +2394,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBA637C-06CC-410C-8E71-3A4C3B33A1DE}">
   <dimension ref="B1:AE75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:31" s="14" customFormat="1" x14ac:dyDescent="0.15">
       <c r="D1" s="14" t="s">
         <v>105</v>
       </c>
@@ -2432,7 +2488,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="2:31" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:31" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B2" s="22"/>
       <c r="E2" s="24">
         <v>44377</v>
@@ -2447,7 +2503,7 @@
         <v>44834</v>
       </c>
     </row>
-    <row r="3" spans="2:31" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:31" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="22"/>
       <c r="E3" s="25">
         <v>11110</v>
@@ -2459,7 +2515,7 @@
         <v>39387</v>
       </c>
     </row>
-    <row r="4" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>55</v>
       </c>
@@ -2476,7 +2532,7 @@
         <v>30.907</v>
       </c>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>56</v>
       </c>
@@ -2493,7 +2549,7 @@
         <v>40.396000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>57</v>
       </c>
@@ -2514,7 +2570,7 @@
         <v>-9.4890000000000008</v>
       </c>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>58</v>
       </c>
@@ -2531,7 +2587,7 @@
         <v>30.745000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>59</v>
       </c>
@@ -2548,7 +2604,7 @@
         <v>10.263</v>
       </c>
     </row>
-    <row r="9" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
@@ -2569,7 +2625,7 @@
         <v>-50.497</v>
       </c>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>63</v>
       </c>
@@ -2586,7 +2642,7 @@
         <v>-0.34</v>
       </c>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>64</v>
       </c>
@@ -2603,7 +2659,7 @@
         <v>4.1820000000000004</v>
       </c>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>65</v>
       </c>
@@ -2620,7 +2676,7 @@
         <v>3.153</v>
       </c>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>61</v>
       </c>
@@ -2637,7 +2693,7 @@
         <v>-0.50800000000000001</v>
       </c>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>62</v>
       </c>
@@ -2654,7 +2710,7 @@
         <v>0.36699999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>75</v>
       </c>
@@ -2675,7 +2731,7 @@
         <v>6.854000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>66</v>
       </c>
@@ -2696,7 +2752,7 @@
         <v>-43.643000000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>67</v>
       </c>
@@ -2713,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
@@ -2734,7 +2790,7 @@
         <v>-43.643000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B19" s="28" t="s">
         <v>69</v>
       </c>
@@ -2755,7 +2811,7 @@
         <v>-0.1301159810917745</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
@@ -2772,7 +2828,7 @@
         <v>335.41613899999999</v>
       </c>
     </row>
-    <row r="22" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
         <v>70</v>
       </c>
@@ -2795,7 +2851,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>71</v>
       </c>
@@ -2818,7 +2874,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
         <v>72</v>
       </c>
@@ -2836,7 +2892,7 @@
         <v>-0.30701782767657815</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
         <v>73</v>
       </c>
@@ -2854,7 +2910,7 @@
         <v>-1.6338369948555342</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
@@ -2872,7 +2928,7 @@
         <v>-1.4120749344808619</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
         <v>67</v>
       </c>
@@ -2890,12 +2946,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B32" s="34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
@@ -2906,7 +2962,7 @@
         <v>71.194000000000003</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>78</v>
       </c>
@@ -2917,7 +2973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>79</v>
       </c>
@@ -2928,7 +2984,7 @@
         <v>1.9770000000000001</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>80</v>
       </c>
@@ -2939,7 +2995,7 @@
         <v>69.228999999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
         <v>81</v>
       </c>
@@ -2950,7 +3006,7 @@
         <v>12.708</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
         <v>82</v>
       </c>
@@ -2963,7 +3019,7 @@
         <v>155.108</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>83</v>
       </c>
@@ -2974,7 +3030,7 @@
         <v>69.84</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>84</v>
       </c>
@@ -2985,7 +3041,7 @@
         <v>13.311999999999999</v>
       </c>
     </row>
-    <row r="41" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B41" s="2" t="s">
         <v>85</v>
       </c>
@@ -2996,7 +3052,7 @@
         <v>4.3380000000000001</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>86</v>
       </c>
@@ -3007,7 +3063,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>87</v>
       </c>
@@ -3020,10 +3076,10 @@
         <v>242.97800000000001</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.15">
       <c r="I44" s="26"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>88</v>
       </c>
@@ -3034,7 +3090,7 @@
         <v>19.728000000000002</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>89</v>
       </c>
@@ -3045,7 +3101,7 @@
         <v>1.4550000000000001</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>90</v>
       </c>
@@ -3056,7 +3112,7 @@
         <v>8.0540000000000003</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
         <v>91</v>
       </c>
@@ -3067,7 +3123,7 @@
         <v>25.094000000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>92</v>
       </c>
@@ -3078,7 +3134,7 @@
         <v>17.927</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
         <v>93</v>
       </c>
@@ -3091,7 +3147,7 @@
         <v>72.25800000000001</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
         <v>94</v>
       </c>
@@ -3102,7 +3158,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
         <v>92</v>
       </c>
@@ -3113,7 +3169,7 @@
         <v>9.1649999999999991</v>
       </c>
     </row>
-    <row r="53" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B53" s="2" t="s">
         <v>95</v>
       </c>
@@ -3124,7 +3180,7 @@
         <v>44.146999999999998</v>
       </c>
     </row>
-    <row r="54" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B54" s="2" t="s">
         <v>96</v>
       </c>
@@ -3135,7 +3191,7 @@
         <v>4.3259999999999996</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
         <v>97</v>
       </c>
@@ -3146,7 +3202,7 @@
         <v>10.795</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
         <v>98</v>
       </c>
@@ -3159,7 +3215,7 @@
         <v>153.49099999999999</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B58" s="1" t="s">
         <v>99</v>
       </c>
@@ -3170,7 +3226,7 @@
         <v>89.486999999999995</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
         <v>100</v>
       </c>
@@ -3183,7 +3239,7 @@
         <v>242.97799999999998</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B61" s="1" t="s">
         <v>101</v>
       </c>
@@ -3196,7 +3252,7 @@
         <v>89.487000000000023</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>102</v>
       </c>
@@ -3209,7 +3265,7 @@
         <v>0.26679396008431194</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
         <v>6</v>
       </c>
@@ -3222,7 +3278,7 @@
         <v>71.194000000000003</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B65" s="1" t="s">
         <v>7</v>
       </c>
@@ -3235,7 +3291,7 @@
         <v>48.472999999999999</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B66" s="1" t="s">
         <v>8</v>
       </c>
@@ -3248,7 +3304,7 @@
         <v>22.721000000000004</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B68" s="1" t="s">
         <v>103</v>
       </c>
@@ -3259,7 +3315,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B69" s="1" t="s">
         <v>5</v>
       </c>
@@ -3272,7 +3328,7 @@
         <v>1029.7275467299999</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B70" s="1" t="s">
         <v>9</v>
       </c>
@@ -3285,7 +3341,7 @@
         <v>1007.0065467299999</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B72" s="1" t="s">
         <v>23</v>
       </c>
@@ -3298,17 +3354,17 @@
         <v>11.507007126509992</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B73" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B74" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B75" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
$VORB UK first launch details
</commit_message>
<xml_diff>
--- a/$VORB.xlsx
+++ b/$VORB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D30C40A-D39D-B749-AD8C-557D195545B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029E8B29-5916-4240-8F46-0609F30CBBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{A3F0CF79-FAAB-4BC8-90D6-455BACE41484}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="150">
   <si>
     <t>$VORB</t>
   </si>
@@ -480,6 +480,12 @@
   </si>
   <si>
     <t>B747-4</t>
+  </si>
+  <si>
+    <t>9th January 2023 Cosmic Girl makes first takeoff for launch of Launcher One from UK soil. First ever space launch from UK soil.</t>
+  </si>
+  <si>
+    <t>LauncherOne launches from UK soil for first ever time</t>
   </si>
 </sst>
 </file>
@@ -682,14 +688,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -708,7 +713,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -716,7 +721,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -737,11 +742,10 @@
     <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -782,7 +786,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,7 +795,7 @@
     <xf numFmtId="17" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -800,61 +804,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -997,7 +995,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1285,7 +1283,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1296,7 +1294,7 @@
   <dimension ref="B2:AA50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:D39"/>
+      <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1315,782 +1313,786 @@
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="H5" s="59" t="s">
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="H5" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="61"/>
-      <c r="V5" s="59" t="s">
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="59"/>
+      <c r="V5" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="W5" s="60"/>
-      <c r="X5" s="60"/>
-      <c r="Y5" s="60"/>
-      <c r="Z5" s="60"/>
-      <c r="AA5" s="61"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="59"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="1">
         <v>2.98</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="7"/>
-      <c r="V6" s="41" t="s">
+      <c r="D6" s="16"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="6"/>
+      <c r="V6" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="7"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="6"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <f>'Financial Model'!J20</f>
         <v>335.41613899999999</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="7"/>
-      <c r="V7" s="47" t="s">
+      <c r="H7" s="33">
+        <v>44927</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="6"/>
+      <c r="V7" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="7"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="6"/>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <f>C6*C7</f>
         <v>999.5400942199999</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="H8" s="35">
-        <v>44866</v>
-      </c>
-      <c r="I8" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="7"/>
-      <c r="V8" s="43" t="s">
+      <c r="D8" s="16"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="6"/>
+      <c r="V8" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="7"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="6"/>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <f>'Financial Model'!J64</f>
         <v>71.194000000000003</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="7"/>
-      <c r="V9" s="42"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="7"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="6"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="6"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <f>'Financial Model'!J65</f>
         <v>48.472999999999999</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="7"/>
-      <c r="V10" s="47" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="6"/>
+      <c r="V10" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="7"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="6"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <f>C9-C10</f>
         <v>22.721000000000004</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="7"/>
-      <c r="V11" s="43" t="s">
+      <c r="H11" s="9"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="6"/>
+      <c r="V11" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="7"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="6"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <f>C8-C11</f>
         <v>976.8190942199999</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="7"/>
-      <c r="V12" s="44" t="s">
+      <c r="D12" s="17"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="6"/>
+      <c r="V12" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="7"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="6"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="H13" s="10"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="7"/>
-      <c r="V13" s="42"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="7"/>
+      <c r="H13" s="33">
+        <v>44866</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="6"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="6"/>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="H14" s="10"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="7"/>
-      <c r="V14" s="41" t="s">
+      <c r="H14" s="9"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="6"/>
+      <c r="V14" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="7"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="6"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="60"/>
-      <c r="D15" s="61"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="7"/>
-      <c r="V15" s="47" t="s">
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="6"/>
+      <c r="V15" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
-      <c r="AA15" s="7"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="6"/>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="45" t="s">
+      <c r="D16" s="61"/>
+      <c r="E16" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="7"/>
-      <c r="V16" s="44" t="s">
+      <c r="H16" s="9"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="6"/>
+      <c r="V16" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="7"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="6"/>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="67"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="7"/>
-      <c r="V17" s="44" t="s">
+      <c r="D17" s="61"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="6"/>
+      <c r="V17" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="6"/>
-      <c r="AA17" s="7"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="6"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="67"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="7"/>
-      <c r="V18" s="44" t="s">
+      <c r="C18" s="60"/>
+      <c r="D18" s="61"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="6"/>
+      <c r="V18" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="7"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="6"/>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="65"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="7"/>
-      <c r="V19" s="44" t="s">
+      <c r="D19" s="67"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="6"/>
+      <c r="V19" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="7"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="6"/>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="H20" s="10"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="7"/>
-      <c r="V20" s="44"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="7"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="6"/>
+      <c r="V20" s="42"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="6"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="H21" s="10"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="7"/>
-      <c r="V21" s="47" t="s">
+      <c r="H21" s="9"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="6"/>
+      <c r="V21" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="7"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="6"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="61"/>
-      <c r="H22" s="35">
+      <c r="C22" s="58"/>
+      <c r="D22" s="59"/>
+      <c r="H22" s="33">
         <v>44531</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="7"/>
-      <c r="V22" s="44" t="s">
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="6"/>
+      <c r="V22" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="W22" s="6"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-      <c r="AA22" s="7"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="6"/>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="66" t="s">
+      <c r="C23" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="67"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="49" t="s">
+      <c r="D23" s="61"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="7"/>
-      <c r="V23" s="40"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
-      <c r="AA23" s="7"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="6"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="6"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="66">
+      <c r="C24" s="60">
         <v>2017</v>
       </c>
-      <c r="D24" s="67"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="7"/>
-      <c r="V24" s="47" t="s">
+      <c r="D24" s="61"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="6"/>
+      <c r="V24" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="7"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="6"/>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="62">
         <v>44560</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="7"/>
-      <c r="V25" s="44" t="s">
+      <c r="D25" s="63"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="6"/>
+      <c r="V25" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
-      <c r="AA25" s="7"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="6"/>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B26" s="10"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="67"/>
-      <c r="H26" s="35">
+      <c r="B26" s="9"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="61"/>
+      <c r="H26" s="33">
         <v>44501</v>
       </c>
-      <c r="I26" s="36" t="s">
+      <c r="I26" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="7"/>
-      <c r="V26" s="40"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="7"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="6"/>
+      <c r="V26" s="38"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="6"/>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B27" s="10"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="67"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="7"/>
-      <c r="V27" s="47" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="61"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="6"/>
+      <c r="V27" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="6"/>
-      <c r="AA27" s="7"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="6"/>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="19">
         <v>39387</v>
       </c>
-      <c r="H28" s="10"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="7"/>
-      <c r="V28" s="44" t="s">
+      <c r="H28" s="9"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="6"/>
+      <c r="V28" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="W28" s="6"/>
-      <c r="X28" s="6"/>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="6"/>
-      <c r="AA28" s="7"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="6"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="68" t="s">
         <v>21</v>
       </c>
       <c r="D29" s="69"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="7"/>
-      <c r="V29" s="48" t="s">
+      <c r="H29" s="9"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="6"/>
+      <c r="V29" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="6"/>
-      <c r="Z29" s="6"/>
-      <c r="AA29" s="7"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="6"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="H30" s="10"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="7"/>
-      <c r="V30" s="40"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="6"/>
-      <c r="AA30" s="7"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="6"/>
+      <c r="V30" s="38"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="6"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="H31" s="10"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="7"/>
-      <c r="V31" s="47" t="s">
+      <c r="H31" s="9"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="6"/>
+      <c r="V31" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
-      <c r="Y31" s="6"/>
-      <c r="Z31" s="6"/>
-      <c r="AA31" s="7"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="6"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B32" s="59" t="s">
+      <c r="B32" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="60"/>
-      <c r="D32" s="61"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="7"/>
-      <c r="V32" s="44" t="s">
+      <c r="C32" s="58"/>
+      <c r="D32" s="59"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="6"/>
+      <c r="V32" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6"/>
-      <c r="AA32" s="7"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="6"/>
     </row>
     <row r="33" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C33" s="70">
@@ -2098,269 +2100,265 @@
         <v>11.16966815537452</v>
       </c>
       <c r="D33" s="71"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="7"/>
-      <c r="V33" s="40"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-      <c r="Z33" s="6"/>
-      <c r="AA33" s="7"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="6"/>
+      <c r="V33" s="38"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="6"/>
     </row>
     <row r="34" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="66"/>
-      <c r="D34" s="67"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="7"/>
-      <c r="V34" s="41" t="s">
+      <c r="C34" s="60"/>
+      <c r="D34" s="61"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="6"/>
+      <c r="V34" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="6"/>
-      <c r="AA34" s="7"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="6"/>
     </row>
     <row r="35" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="67"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
-      <c r="S35" s="7"/>
-      <c r="V35" s="42" t="s">
+      <c r="C35" s="60"/>
+      <c r="D35" s="61"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="6"/>
+      <c r="V35" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="W35" s="6"/>
-      <c r="X35" s="6"/>
-      <c r="Y35" s="6"/>
-      <c r="Z35" s="6"/>
-      <c r="AA35" s="7"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="6"/>
     </row>
     <row r="36" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="64"/>
-      <c r="D36" s="65"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="9"/>
-      <c r="V36" s="46" t="s">
+      <c r="C36" s="66"/>
+      <c r="D36" s="67"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="8"/>
+      <c r="V36" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-      <c r="AA36" s="9"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="8"/>
     </row>
     <row r="39" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B39" s="59" t="s">
+      <c r="B39" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="60"/>
-      <c r="D39" s="61"/>
-      <c r="V39" s="59" t="s">
+      <c r="C39" s="58"/>
+      <c r="D39" s="59"/>
+      <c r="V39" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="W39" s="60"/>
-      <c r="X39" s="60"/>
-      <c r="Y39" s="60"/>
-      <c r="Z39" s="60"/>
-      <c r="AA39" s="61"/>
+      <c r="W39" s="58"/>
+      <c r="X39" s="58"/>
+      <c r="Y39" s="58"/>
+      <c r="Z39" s="58"/>
+      <c r="AA39" s="59"/>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="62" t="s">
+      <c r="C40" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="63"/>
-      <c r="V40" s="50"/>
-      <c r="W40" s="6"/>
-      <c r="X40" s="6"/>
-      <c r="Y40" s="6"/>
-      <c r="Z40" s="6"/>
-      <c r="AA40" s="7"/>
+      <c r="D40" s="65"/>
+      <c r="V40" s="49">
+        <v>44927</v>
+      </c>
+      <c r="W40" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="6"/>
     </row>
     <row r="41" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B41" s="10"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="31"/>
-      <c r="V41" s="50"/>
-      <c r="W41" s="6"/>
-      <c r="X41" s="6"/>
-      <c r="Y41" s="6"/>
-      <c r="Z41" s="6"/>
-      <c r="AA41" s="7"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29"/>
+      <c r="V41" s="48"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5"/>
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="6"/>
     </row>
     <row r="42" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B42" s="10"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="31"/>
-      <c r="V42" s="51">
+      <c r="B42" s="9"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="29"/>
+      <c r="V42" s="49">
         <v>44562</v>
       </c>
-      <c r="W42" s="6" t="s">
+      <c r="W42" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="X42" s="6"/>
-      <c r="Y42" s="6"/>
-      <c r="Z42" s="6"/>
-      <c r="AA42" s="7"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="6"/>
     </row>
     <row r="43" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B43" s="11"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="33"/>
-      <c r="J43" s="56"/>
-      <c r="V43" s="50"/>
-      <c r="W43" s="6"/>
-      <c r="X43" s="6"/>
-      <c r="Y43" s="6"/>
-      <c r="Z43" s="6"/>
-      <c r="AA43" s="7"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="31"/>
+      <c r="J43" s="54"/>
+      <c r="V43" s="48"/>
+      <c r="W43" s="5"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="5"/>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="6"/>
     </row>
     <row r="44" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="V44" s="51">
+      <c r="V44" s="49">
         <v>44348</v>
       </c>
-      <c r="W44" s="6" t="s">
+      <c r="W44" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="X44" s="6"/>
-      <c r="Y44" s="6"/>
-      <c r="Z44" s="6"/>
-      <c r="AA44" s="7"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="6"/>
     </row>
     <row r="45" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="V45" s="50"/>
-      <c r="W45" s="6"/>
-      <c r="X45" s="6"/>
-      <c r="Y45" s="6"/>
-      <c r="Z45" s="6"/>
-      <c r="AA45" s="7"/>
+      <c r="V45" s="48"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="6"/>
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="60"/>
-      <c r="D46" s="61"/>
-      <c r="V46" s="51">
+      <c r="C46" s="58"/>
+      <c r="D46" s="59"/>
+      <c r="V46" s="49">
         <v>44197</v>
       </c>
-      <c r="W46" s="6" t="s">
+      <c r="W46" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="X46" s="6"/>
-      <c r="Y46" s="6"/>
-      <c r="Z46" s="6"/>
-      <c r="AA46" s="7"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="6"/>
     </row>
     <row r="47" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B47" s="74" t="s">
+      <c r="B47" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="C47" s="57" t="s">
+      <c r="C47" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D47" s="7"/>
-      <c r="V47" s="50"/>
-      <c r="W47" s="52" t="s">
+      <c r="D47" s="6"/>
+      <c r="V47" s="48"/>
+      <c r="W47" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="X47" s="6"/>
-      <c r="Y47" s="6"/>
-      <c r="Z47" s="6"/>
-      <c r="AA47" s="7"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="6"/>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B48" s="50"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="7"/>
-      <c r="V48" s="50"/>
-      <c r="W48" s="6"/>
-      <c r="X48" s="6"/>
-      <c r="Y48" s="6"/>
-      <c r="Z48" s="6"/>
-      <c r="AA48" s="7"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="6"/>
+      <c r="V48" s="48"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="6"/>
     </row>
     <row r="49" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B49" s="50"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="7"/>
-      <c r="V49" s="53">
+      <c r="B49" s="48"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="6"/>
+      <c r="V49" s="51">
         <v>43952</v>
       </c>
-      <c r="W49" s="8" t="s">
+      <c r="W49" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="X49" s="54"/>
-      <c r="Y49" s="54"/>
-      <c r="Z49" s="54"/>
-      <c r="AA49" s="55"/>
+      <c r="X49" s="52"/>
+      <c r="Y49" s="52"/>
+      <c r="Z49" s="52"/>
+      <c r="AA49" s="53"/>
     </row>
     <row r="50" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B50" s="75"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="9"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
     <mergeCell ref="V5:AA5"/>
     <mergeCell ref="V39:AA39"/>
     <mergeCell ref="B39:D39"/>
@@ -2377,10 +2375,18 @@
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{D9BC7303-6CA5-439B-B622-1349F7C34E60}"/>
-    <hyperlink ref="I8" r:id="rId2" xr:uid="{E39DBCF5-486C-40D8-8DE7-3B1B2093CF5E}"/>
+    <hyperlink ref="I13" r:id="rId2" xr:uid="{E39DBCF5-486C-40D8-8DE7-3B1B2093CF5E}"/>
     <hyperlink ref="C40:D40" r:id="rId3" display="Link" xr:uid="{2B0F95BB-3327-4579-B7A8-ECBB8C4B69A6}"/>
     <hyperlink ref="I26" r:id="rId4" xr:uid="{FD0C5381-0521-4F12-85A8-E23C70816062}"/>
     <hyperlink ref="B47" r:id="rId5" location="flightPageActivityLog" xr:uid="{0D1432A5-D70D-A641-98CE-1CDD0A717403}"/>
@@ -2408,110 +2414,110 @@
     <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" s="14" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="D1" s="14" t="s">
+    <row r="1" spans="2:31" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="D1" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Y1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AA1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AB1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AC1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AD1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AE1" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="2:31" s="23" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="22"/>
-      <c r="E2" s="24">
+    <row r="2" spans="2:31" s="22" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="21"/>
+      <c r="E2" s="23">
         <v>44377</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="23">
         <v>44469</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="23">
         <v>44742</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="23">
         <v>44834</v>
       </c>
     </row>
-    <row r="3" spans="2:31" s="23" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="22"/>
-      <c r="E3" s="25">
+    <row r="3" spans="2:31" s="22" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="21"/>
+      <c r="E3" s="24">
         <v>11110</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="24">
         <v>41122</v>
       </c>
-      <c r="J3" s="25">
+      <c r="J3" s="24">
         <v>39387</v>
       </c>
     </row>
@@ -2519,16 +2525,16 @@
       <c r="B4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="36">
         <v>1.6930000000000001</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="25">
         <v>2E-3</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="25">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="25">
         <v>30.907</v>
       </c>
     </row>
@@ -2536,16 +2542,16 @@
       <c r="B5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="35">
         <v>14.292</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="14">
         <v>8.6969999999999992</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="14">
         <v>3.427</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="14">
         <v>40.396000000000001</v>
       </c>
     </row>
@@ -2553,19 +2559,19 @@
       <c r="B6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="36">
         <f>E4-E5</f>
         <v>-12.599</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="25">
         <f>F4-F5</f>
         <v>-8.6949999999999985</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="25">
         <f>I4-I5</f>
         <v>-3.4220000000000002</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="25">
         <f>J4-J5</f>
         <v>-9.4890000000000008</v>
       </c>
@@ -2574,16 +2580,16 @@
       <c r="B7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="35">
         <v>20.48</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="14">
         <v>27.163</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="14">
         <v>27.844999999999999</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="14">
         <v>30.745000000000001</v>
       </c>
     </row>
@@ -2591,16 +2597,16 @@
       <c r="B8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="35">
         <v>11.616</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="14">
         <v>9.0350000000000001</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="14">
         <v>9.1349999999999998</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="14">
         <v>10.263</v>
       </c>
     </row>
@@ -2608,19 +2614,19 @@
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="36">
         <f>E6-E7-E8</f>
         <v>-44.695</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="25">
         <f>F6-F7-F8</f>
         <v>-44.893000000000001</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="25">
         <f>I6-I7-I8</f>
         <v>-40.402000000000001</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="25">
         <f>J6-J7-J8</f>
         <v>-50.497</v>
       </c>
@@ -2629,16 +2635,16 @@
       <c r="B10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E10" s="35">
         <v>0</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="14">
         <v>4.8520000000000003</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="14">
         <v>-4.6349999999999998</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="14">
         <v>-0.34</v>
       </c>
     </row>
@@ -2646,16 +2652,16 @@
       <c r="B11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="35">
         <v>0</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="14">
         <v>0</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="14">
         <v>11.68</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="14">
         <v>4.1820000000000004</v>
       </c>
     </row>
@@ -2663,16 +2669,16 @@
       <c r="B12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="35">
         <v>0</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="14">
         <v>0</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="14">
         <v>0</v>
       </c>
-      <c r="J12" s="26">
+      <c r="J12" s="14">
         <v>3.153</v>
       </c>
     </row>
@@ -2680,16 +2686,16 @@
       <c r="B13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="37">
+      <c r="E13" s="35">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="14">
         <v>-6.0000000000000001E-3</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="14">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="14">
         <v>-0.50800000000000001</v>
       </c>
     </row>
@@ -2697,16 +2703,16 @@
       <c r="B14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="35">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="14">
         <v>1.4570000000000001</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="14">
         <v>0.121</v>
       </c>
-      <c r="J14" s="26">
+      <c r="J14" s="14">
         <v>0.36699999999999999</v>
       </c>
     </row>
@@ -2714,19 +2720,19 @@
       <c r="B15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15" s="35">
         <f>SUM(E10:E14)</f>
         <v>4.7E-2</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="14">
         <f>SUM(F10:F14)</f>
         <v>6.3029999999999999</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I15" s="14">
         <f>SUM(I10:I14)</f>
         <v>7.1140000000000008</v>
       </c>
-      <c r="J15" s="26">
+      <c r="J15" s="14">
         <f>SUM(J10:J14)</f>
         <v>6.854000000000001</v>
       </c>
@@ -2735,19 +2741,19 @@
       <c r="B16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="35">
         <f>E9+E15</f>
         <v>-44.648000000000003</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="14">
         <f>F9+F15</f>
         <v>-38.590000000000003</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="14">
         <f>I9+I15</f>
         <v>-33.287999999999997</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="14">
         <f>J9+J15</f>
         <v>-43.643000000000001</v>
       </c>
@@ -2756,16 +2762,16 @@
       <c r="B17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="37">
+      <c r="E17" s="35">
         <v>0</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="14">
         <v>0</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="14">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2773,40 +2779,40 @@
       <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="36">
         <f>E16-E17</f>
         <v>-44.648000000000003</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="25">
         <f>F16-F17</f>
         <v>-38.590000000000003</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="25">
         <f>I16-I17</f>
         <v>-33.291999999999994</v>
       </c>
-      <c r="J18" s="27">
+      <c r="J18" s="25">
         <f>J16-J17</f>
         <v>-43.643000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:10" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="28" t="s">
+    <row r="19" spans="2:10" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="26">
         <f>E18/E20</f>
         <v>-0.15717012057874949</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="26">
         <f>F18/F20</f>
         <v>-0.13120292155961089</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I19" s="26">
         <f>I18/I20</f>
         <v>-9.9390398787167239E-2</v>
       </c>
-      <c r="J19" s="28">
+      <c r="J19" s="26">
         <f>J18/J20</f>
         <v>-0.1301159810917745</v>
       </c>
@@ -2815,16 +2821,16 @@
       <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="14">
         <v>284.07435099999998</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="14">
         <v>294.124548</v>
       </c>
-      <c r="I20" s="37">
+      <c r="I20" s="35">
         <v>334.96193199999999</v>
       </c>
-      <c r="J20" s="26">
+      <c r="J20" s="14">
         <v>335.41613899999999</v>
       </c>
     </row>
@@ -2832,22 +2838,22 @@
       <c r="B22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="13" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2855,22 +2861,22 @@
       <c r="B23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="13" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2878,16 +2884,16 @@
       <c r="B25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="27">
         <f>J6/J4</f>
         <v>-0.30701782767657815</v>
       </c>
@@ -2896,16 +2902,16 @@
       <c r="B26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J26" s="29">
+      <c r="J26" s="27">
         <f>J9/J4</f>
         <v>-1.6338369948555342</v>
       </c>
@@ -2914,16 +2920,16 @@
       <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J27" s="29">
+      <c r="J27" s="27">
         <f>J18/J4</f>
         <v>-1.4120749344808619</v>
       </c>
@@ -2932,22 +2938,22 @@
       <c r="B28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J28" s="29">
+      <c r="J28" s="27">
         <f>J17/J16</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="32" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2955,10 +2961,10 @@
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="27">
+      <c r="I33" s="25">
         <v>122.072</v>
       </c>
-      <c r="J33" s="27">
+      <c r="J33" s="25">
         <v>71.194000000000003</v>
       </c>
     </row>
@@ -2966,10 +2972,10 @@
       <c r="B34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I34" s="26">
+      <c r="I34" s="14">
         <v>0.82799999999999996</v>
       </c>
-      <c r="J34" s="26">
+      <c r="J34" s="14">
         <v>0</v>
       </c>
     </row>
@@ -2977,10 +2983,10 @@
       <c r="B35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I35" s="26">
+      <c r="I35" s="14">
         <v>11.263</v>
       </c>
-      <c r="J35" s="26">
+      <c r="J35" s="14">
         <v>1.9770000000000001</v>
       </c>
     </row>
@@ -2988,10 +2994,10 @@
       <c r="B36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I36" s="26">
+      <c r="I36" s="14">
         <v>66.528999999999996</v>
       </c>
-      <c r="J36" s="26">
+      <c r="J36" s="14">
         <v>69.228999999999999</v>
       </c>
     </row>
@@ -2999,10 +3005,10 @@
       <c r="B37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I37" s="26">
+      <c r="I37" s="14">
         <v>15.122</v>
       </c>
-      <c r="J37" s="26">
+      <c r="J37" s="14">
         <v>12.708</v>
       </c>
     </row>
@@ -3010,11 +3016,11 @@
       <c r="B38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I38" s="26">
+      <c r="I38" s="14">
         <f>SUM(I33:I37)</f>
         <v>215.81400000000002</v>
       </c>
-      <c r="J38" s="26">
+      <c r="J38" s="14">
         <f>SUM(J33:J37)</f>
         <v>155.108</v>
       </c>
@@ -3023,10 +3029,10 @@
       <c r="B39" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I39" s="26">
+      <c r="I39" s="14">
         <v>65.837999999999994</v>
       </c>
-      <c r="J39" s="26">
+      <c r="J39" s="14">
         <v>69.84</v>
       </c>
     </row>
@@ -3034,10 +3040,10 @@
       <c r="B40" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I40" s="26">
+      <c r="I40" s="14">
         <v>12.986000000000001</v>
       </c>
-      <c r="J40" s="26">
+      <c r="J40" s="14">
         <v>13.311999999999999</v>
       </c>
     </row>
@@ -3045,10 +3051,10 @@
       <c r="B41" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I41" s="27">
+      <c r="I41" s="25">
         <v>4.6779999999999999</v>
       </c>
-      <c r="J41" s="27">
+      <c r="J41" s="25">
         <v>4.3380000000000001</v>
       </c>
     </row>
@@ -3056,10 +3062,10 @@
       <c r="B42" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I42" s="26">
+      <c r="I42" s="14">
         <v>1.4039999999999999</v>
       </c>
-      <c r="J42" s="26">
+      <c r="J42" s="14">
         <v>0.38</v>
       </c>
     </row>
@@ -3067,26 +3073,26 @@
       <c r="B43" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I43" s="26">
+      <c r="I43" s="14">
         <f>I38+SUM(I39:I42)</f>
         <v>300.72000000000003</v>
       </c>
-      <c r="J43" s="26">
+      <c r="J43" s="14">
         <f>J38+SUM(J39:J42)</f>
         <v>242.97800000000001</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.15">
-      <c r="I44" s="26"/>
+      <c r="I44" s="14"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I45" s="26">
+      <c r="I45" s="14">
         <v>9.0640000000000001</v>
       </c>
-      <c r="J45" s="26">
+      <c r="J45" s="14">
         <v>19.728000000000002</v>
       </c>
     </row>
@@ -3094,10 +3100,10 @@
       <c r="B46" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I46" s="26">
+      <c r="I46" s="14">
         <v>1.3480000000000001</v>
       </c>
-      <c r="J46" s="26">
+      <c r="J46" s="14">
         <v>1.4550000000000001</v>
       </c>
     </row>
@@ -3105,10 +3111,10 @@
       <c r="B47" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I47" s="26">
+      <c r="I47" s="14">
         <v>4.75</v>
       </c>
-      <c r="J47" s="26">
+      <c r="J47" s="14">
         <v>8.0540000000000003</v>
       </c>
     </row>
@@ -3116,10 +3122,10 @@
       <c r="B48" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I48" s="26">
+      <c r="I48" s="14">
         <v>22.611000000000001</v>
       </c>
-      <c r="J48" s="26">
+      <c r="J48" s="14">
         <v>25.094000000000001</v>
       </c>
     </row>
@@ -3127,10 +3133,10 @@
       <c r="B49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I49" s="26">
+      <c r="I49" s="14">
         <v>37.329000000000001</v>
       </c>
-      <c r="J49" s="26">
+      <c r="J49" s="14">
         <v>17.927</v>
       </c>
     </row>
@@ -3138,11 +3144,11 @@
       <c r="B50" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="I50" s="26">
+      <c r="I50" s="14">
         <f>SUM(I45:I49)</f>
         <v>75.102000000000004</v>
       </c>
-      <c r="J50" s="26">
+      <c r="J50" s="14">
         <f>SUM(J45:J49)</f>
         <v>72.25800000000001</v>
       </c>
@@ -3151,10 +3157,10 @@
       <c r="B51" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I51" s="26">
+      <c r="I51" s="14">
         <v>12.595000000000001</v>
       </c>
-      <c r="J51" s="26">
+      <c r="J51" s="14">
         <v>12.8</v>
       </c>
     </row>
@@ -3162,10 +3168,10 @@
       <c r="B52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="26">
+      <c r="I52" s="14">
         <v>20.753</v>
       </c>
-      <c r="J52" s="26">
+      <c r="J52" s="14">
         <v>9.1649999999999991</v>
       </c>
     </row>
@@ -3173,10 +3179,10 @@
       <c r="B53" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I53" s="27">
+      <c r="I53" s="25">
         <v>50</v>
       </c>
-      <c r="J53" s="27">
+      <c r="J53" s="25">
         <v>44.146999999999998</v>
       </c>
     </row>
@@ -3184,10 +3190,10 @@
       <c r="B54" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="I54" s="27">
+      <c r="I54" s="25">
         <v>8.5079999999999991</v>
       </c>
-      <c r="J54" s="27">
+      <c r="J54" s="25">
         <v>4.3259999999999996</v>
       </c>
     </row>
@@ -3195,10 +3201,10 @@
       <c r="B55" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I55" s="26">
+      <c r="I55" s="14">
         <v>9.6449999999999996</v>
       </c>
-      <c r="J55" s="26">
+      <c r="J55" s="14">
         <v>10.795</v>
       </c>
     </row>
@@ -3206,11 +3212,11 @@
       <c r="B56" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I56" s="26">
+      <c r="I56" s="14">
         <f>I50+SUM(I51:I55)</f>
         <v>176.60300000000001</v>
       </c>
-      <c r="J56" s="26">
+      <c r="J56" s="14">
         <f>J50+SUM(J51:J55)</f>
         <v>153.49099999999999</v>
       </c>
@@ -3219,10 +3225,10 @@
       <c r="B58" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="I58" s="26">
+      <c r="I58" s="14">
         <v>124.117</v>
       </c>
-      <c r="J58" s="26">
+      <c r="J58" s="14">
         <v>89.486999999999995</v>
       </c>
     </row>
@@ -3230,11 +3236,11 @@
       <c r="B59" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="I59" s="26">
+      <c r="I59" s="14">
         <f>I58+I56</f>
         <v>300.72000000000003</v>
       </c>
-      <c r="J59" s="26">
+      <c r="J59" s="14">
         <f>J58+J56</f>
         <v>242.97799999999998</v>
       </c>
@@ -3243,11 +3249,11 @@
       <c r="B61" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I61" s="26">
+      <c r="I61" s="14">
         <f>I43-I56</f>
         <v>124.11700000000002</v>
       </c>
-      <c r="J61" s="26">
+      <c r="J61" s="14">
         <f t="shared" ref="J61" si="0">J43-J56</f>
         <v>89.487000000000023</v>
       </c>
@@ -3269,11 +3275,11 @@
       <c r="B64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I64" s="26">
+      <c r="I64" s="14">
         <f>I33</f>
         <v>122.072</v>
       </c>
-      <c r="J64" s="26">
+      <c r="J64" s="14">
         <f t="shared" ref="J64" si="2">J33</f>
         <v>71.194000000000003</v>
       </c>
@@ -3282,11 +3288,11 @@
       <c r="B65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I65" s="26">
+      <c r="I65" s="14">
         <f>I53+I54</f>
         <v>58.507999999999996</v>
       </c>
-      <c r="J65" s="26">
+      <c r="J65" s="14">
         <f t="shared" ref="J65" si="3">J53+J54</f>
         <v>48.472999999999999</v>
       </c>
@@ -3295,11 +3301,11 @@
       <c r="B66" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I66" s="26">
+      <c r="I66" s="14">
         <f>I64-I65</f>
         <v>63.564000000000007</v>
       </c>
-      <c r="J66" s="26">
+      <c r="J66" s="14">
         <f t="shared" ref="J66" si="4">J64-J65</f>
         <v>22.721000000000004</v>
       </c>
@@ -3319,11 +3325,11 @@
       <c r="B69" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I69" s="26">
+      <c r="I69" s="14">
         <f>I68*I20</f>
         <v>1282.9041995600001</v>
       </c>
-      <c r="J69" s="26">
+      <c r="J69" s="14">
         <f t="shared" ref="J69" si="5">J68*J20</f>
         <v>1029.7275467299999</v>
       </c>
@@ -3332,11 +3338,11 @@
       <c r="B70" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I70" s="26">
+      <c r="I70" s="14">
         <f>I69-I66</f>
         <v>1219.34019956</v>
       </c>
-      <c r="J70" s="26">
+      <c r="J70" s="14">
         <f t="shared" ref="J70" si="6">J69-J66</f>
         <v>1007.0065467299999</v>
       </c>
@@ -3345,11 +3351,11 @@
       <c r="B72" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="39">
+      <c r="I72" s="37">
         <f>I68/I62</f>
         <v>10.336248858415848</v>
       </c>
-      <c r="J72" s="39">
+      <c r="J72" s="37">
         <f t="shared" ref="J72" si="7">J68/J62</f>
         <v>11.507007126509992</v>
       </c>

</xml_diff>

<commit_message>
$VORB update following failed launch
</commit_message>
<xml_diff>
--- a/$VORB.xlsx
+++ b/$VORB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029E8B29-5916-4240-8F46-0609F30CBBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484C61F7-A52A-3C47-8CD7-BC7472069D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{A3F0CF79-FAAB-4BC8-90D6-455BACE41484}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="152">
   <si>
     <t>$VORB</t>
   </si>
@@ -486,6 +486,12 @@
   </si>
   <si>
     <t>LauncherOne launches from UK soil for first ever time</t>
+  </si>
+  <si>
+    <t>FAILED TO ACHIEVE INTENDED ORBIT</t>
+  </si>
+  <si>
+    <t>Launch fails to reach intended orbit after much confusion, very poor communication &amp; disorganised livestream &amp; media team</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,6 +571,13 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -688,7 +701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -819,42 +832,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="15" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1294,7 +1311,7 @@
   <dimension ref="B2:AA50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V41" sqref="V41"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1416,7 +1433,9 @@
       </c>
       <c r="D8" s="16"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="73" t="s">
+        <v>151</v>
+      </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1637,10 +1656,10 @@
       <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="61"/>
+      <c r="D16" s="65"/>
       <c r="E16" s="43" t="s">
         <v>114</v>
       </c>
@@ -1669,10 +1688,10 @@
       <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="61"/>
+      <c r="D17" s="65"/>
       <c r="H17" s="9"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1698,8 +1717,8 @@
       <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="61"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="65"/>
       <c r="H18" s="9"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1725,10 +1744,10 @@
       <c r="B19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="67"/>
+      <c r="D19" s="63"/>
       <c r="H19" s="9"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1827,10 +1846,10 @@
       <c r="B23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="61"/>
+      <c r="D23" s="65"/>
       <c r="H23" s="9"/>
       <c r="I23" s="47" t="s">
         <v>124</v>
@@ -1856,10 +1875,10 @@
       <c r="B24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="60">
+      <c r="C24" s="64">
         <v>2017</v>
       </c>
-      <c r="D24" s="61"/>
+      <c r="D24" s="65"/>
       <c r="H24" s="9"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -1885,10 +1904,10 @@
       <c r="B25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="62">
+      <c r="C25" s="70">
         <v>44560</v>
       </c>
-      <c r="D25" s="63"/>
+      <c r="D25" s="71"/>
       <c r="H25" s="9"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -1912,8 +1931,8 @@
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B26" s="9"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="61"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="65"/>
       <c r="H26" s="33">
         <v>44501</v>
       </c>
@@ -1939,8 +1958,8 @@
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B27" s="9"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="61"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="65"/>
       <c r="H27" s="9"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -1997,10 +2016,10 @@
       <c r="B29" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="68" t="s">
+      <c r="C29" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="69"/>
+      <c r="D29" s="67"/>
       <c r="H29" s="9"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -2095,11 +2114,11 @@
       <c r="B33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="70">
+      <c r="C33" s="68">
         <f>C6/'Financial Model'!J62</f>
         <v>11.16966815537452</v>
       </c>
-      <c r="D33" s="71"/>
+      <c r="D33" s="69"/>
       <c r="H33" s="9"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -2123,8 +2142,8 @@
       <c r="B34" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="61"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="65"/>
       <c r="H34" s="9"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -2150,8 +2169,8 @@
       <c r="B35" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="61"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="65"/>
       <c r="H35" s="9"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -2177,8 +2196,8 @@
       <c r="B36" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="66"/>
-      <c r="D36" s="67"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="63"/>
       <c r="H36" s="10"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
@@ -2219,10 +2238,10 @@
       <c r="B40" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="64" t="s">
+      <c r="C40" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="65"/>
+      <c r="D40" s="61"/>
       <c r="V40" s="49">
         <v>44927</v>
       </c>
@@ -2239,7 +2258,9 @@
       <c r="C41" s="28"/>
       <c r="D41" s="29"/>
       <c r="V41" s="48"/>
-      <c r="W41" s="5"/>
+      <c r="W41" s="72" t="s">
+        <v>150</v>
+      </c>
       <c r="X41" s="5"/>
       <c r="Y41" s="5"/>
       <c r="Z41" s="5"/>
@@ -2359,6 +2380,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="V5:AA5"/>
     <mergeCell ref="V39:AA39"/>
     <mergeCell ref="B39:D39"/>
@@ -2375,14 +2404,6 @@
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{D9BC7303-6CA5-439B-B622-1349F7C34E60}"/>

</xml_diff>

<commit_message>
$VORB more details following launch failure
</commit_message>
<xml_diff>
--- a/$VORB.xlsx
+++ b/$VORB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484C61F7-A52A-3C47-8CD7-BC7472069D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4D6F4E-35CD-0440-9C78-42A3D0090DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{A3F0CF79-FAAB-4BC8-90D6-455BACE41484}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="154">
   <si>
     <t>$VORB</t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>Launch fails to reach intended orbit after much confusion, very poor communication &amp; disorganised livestream &amp; media team</t>
+  </si>
+  <si>
+    <t>Share price crashes 20%, stabalises to a close of -13.99%</t>
+  </si>
+  <si>
+    <t>Virgin Orbit turn to Richard Branson's Virgin Group for a $25 million cash injection</t>
   </si>
 </sst>
 </file>
@@ -823,6 +829,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -832,6 +842,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -844,12 +866,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -862,16 +878,6 @@
     <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1311,7 +1317,7 @@
   <dimension ref="B2:AA50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1330,40 +1336,40 @@
       </c>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="H5" s="57" t="s">
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="H5" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="59"/>
-      <c r="V5" s="57" t="s">
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="61"/>
+      <c r="V5" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="W5" s="58"/>
-      <c r="X5" s="58"/>
-      <c r="Y5" s="58"/>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="59"/>
+      <c r="W5" s="60"/>
+      <c r="X5" s="60"/>
+      <c r="Y5" s="60"/>
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="61"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>2.98</v>
+        <v>1.66</v>
       </c>
       <c r="D6" s="16"/>
       <c r="H6" s="9"/>
@@ -1398,12 +1404,8 @@
       <c r="D7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="33">
-        <v>44927</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>148</v>
-      </c>
+      <c r="H7" s="33"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -1429,13 +1431,11 @@
       </c>
       <c r="C8" s="14">
         <f>C6*C7</f>
-        <v>999.5400942199999</v>
+        <v>556.79079073999992</v>
       </c>
       <c r="D8" s="16"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="73" t="s">
-        <v>151</v>
-      </c>
+      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1466,8 +1466,12 @@
       <c r="D9" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="5"/>
+      <c r="H9" s="33">
+        <v>44927</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -1497,7 +1501,9 @@
         <v>50</v>
       </c>
       <c r="H10" s="9"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="58" t="s">
+        <v>151</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1529,7 +1535,9 @@
         <v>50</v>
       </c>
       <c r="H11" s="9"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="58" t="s">
+        <v>152</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -1555,7 +1563,7 @@
       </c>
       <c r="C12" s="15">
         <f>C8-C11</f>
-        <v>976.8190942199999</v>
+        <v>534.06979073999992</v>
       </c>
       <c r="D12" s="17"/>
       <c r="H12" s="9"/>
@@ -1626,13 +1634,17 @@
       <c r="AA14" s="6"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="5"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="61"/>
+      <c r="H15" s="33">
+        <v>44866</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1656,10 +1668,10 @@
       <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="65"/>
+      <c r="D16" s="63"/>
       <c r="E16" s="43" t="s">
         <v>114</v>
       </c>
@@ -1688,12 +1700,16 @@
       <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="5"/>
+      <c r="D17" s="63"/>
+      <c r="H17" s="33">
+        <v>44531</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -1717,10 +1733,12 @@
       <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="65"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="5"/>
+      <c r="I18" s="47" t="s">
+        <v>124</v>
+      </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -1744,10 +1762,10 @@
       <c r="B19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="63"/>
+      <c r="D19" s="69"/>
       <c r="H19" s="9"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1790,8 +1808,12 @@
       <c r="AA20" s="6"/>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="H21" s="9"/>
-      <c r="I21" s="5"/>
+      <c r="H21" s="33">
+        <v>44501</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>144</v>
+      </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -1812,17 +1834,13 @@
       <c r="AA21" s="6"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="58"/>
-      <c r="D22" s="59"/>
-      <c r="H22" s="33">
-        <v>44531</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="C22" s="60"/>
+      <c r="D22" s="61"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -1846,14 +1864,12 @@
       <c r="B23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="65"/>
+      <c r="D23" s="63"/>
       <c r="H23" s="9"/>
-      <c r="I23" s="47" t="s">
-        <v>124</v>
-      </c>
+      <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -1875,10 +1891,10 @@
       <c r="B24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="64">
+      <c r="C24" s="62">
         <v>2017</v>
       </c>
-      <c r="D24" s="65"/>
+      <c r="D24" s="63"/>
       <c r="H24" s="9"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -1904,10 +1920,10 @@
       <c r="B25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="70">
+      <c r="C25" s="64">
         <v>44560</v>
       </c>
-      <c r="D25" s="71"/>
+      <c r="D25" s="65"/>
       <c r="H25" s="9"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -1931,14 +1947,10 @@
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B26" s="9"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="65"/>
-      <c r="H26" s="33">
-        <v>44501</v>
-      </c>
-      <c r="I26" s="34" t="s">
-        <v>144</v>
-      </c>
+      <c r="C26" s="62"/>
+      <c r="D26" s="63"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -1958,8 +1970,8 @@
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B27" s="9"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="65"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="63"/>
       <c r="H27" s="9"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -2016,10 +2028,10 @@
       <c r="B29" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="67"/>
+      <c r="D29" s="71"/>
       <c r="H29" s="9"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -2084,11 +2096,11 @@
       <c r="AA31" s="6"/>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B32" s="57" t="s">
+      <c r="B32" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="61"/>
       <c r="H32" s="9"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -2114,11 +2126,11 @@
       <c r="B33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="68">
+      <c r="C33" s="72">
         <f>C6/'Financial Model'!J62</f>
-        <v>11.16966815537452</v>
-      </c>
-      <c r="D33" s="69"/>
+        <v>6.2220299120542624</v>
+      </c>
+      <c r="D33" s="73"/>
       <c r="H33" s="9"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -2142,8 +2154,8 @@
       <c r="B34" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="64"/>
-      <c r="D34" s="65"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="63"/>
       <c r="H34" s="9"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -2169,8 +2181,8 @@
       <c r="B35" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="64"/>
-      <c r="D35" s="65"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="63"/>
       <c r="H35" s="9"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -2196,8 +2208,8 @@
       <c r="B36" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="62"/>
-      <c r="D36" s="63"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="69"/>
       <c r="H36" s="10"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
@@ -2220,28 +2232,28 @@
       <c r="AA36" s="8"/>
     </row>
     <row r="39" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B39" s="57" t="s">
+      <c r="B39" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="59"/>
-      <c r="V39" s="57" t="s">
+      <c r="C39" s="60"/>
+      <c r="D39" s="61"/>
+      <c r="V39" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="W39" s="58"/>
-      <c r="X39" s="58"/>
-      <c r="Y39" s="58"/>
-      <c r="Z39" s="58"/>
-      <c r="AA39" s="59"/>
+      <c r="W39" s="60"/>
+      <c r="X39" s="60"/>
+      <c r="Y39" s="60"/>
+      <c r="Z39" s="60"/>
+      <c r="AA39" s="61"/>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.15">
       <c r="B40" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="60" t="s">
+      <c r="C40" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="61"/>
+      <c r="D40" s="67"/>
       <c r="V40" s="49">
         <v>44927</v>
       </c>
@@ -2258,7 +2270,7 @@
       <c r="C41" s="28"/>
       <c r="D41" s="29"/>
       <c r="V41" s="48"/>
-      <c r="W41" s="72" t="s">
+      <c r="W41" s="57" t="s">
         <v>150</v>
       </c>
       <c r="X41" s="5"/>
@@ -2314,11 +2326,11 @@
       <c r="AA45" s="6"/>
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.15">
-      <c r="B46" s="57" t="s">
+      <c r="B46" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="58"/>
-      <c r="D46" s="59"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="61"/>
       <c r="V46" s="49">
         <v>44197</v>
       </c>
@@ -2380,14 +2392,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
     <mergeCell ref="V5:AA5"/>
     <mergeCell ref="V39:AA39"/>
     <mergeCell ref="B39:D39"/>
@@ -2404,12 +2408,20 @@
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{D9BC7303-6CA5-439B-B622-1349F7C34E60}"/>
     <hyperlink ref="I13" r:id="rId2" xr:uid="{E39DBCF5-486C-40D8-8DE7-3B1B2093CF5E}"/>
     <hyperlink ref="C40:D40" r:id="rId3" display="Link" xr:uid="{2B0F95BB-3327-4579-B7A8-ECBB8C4B69A6}"/>
-    <hyperlink ref="I26" r:id="rId4" xr:uid="{FD0C5381-0521-4F12-85A8-E23C70816062}"/>
+    <hyperlink ref="I21" r:id="rId4" xr:uid="{FD0C5381-0521-4F12-85A8-E23C70816062}"/>
     <hyperlink ref="B47" r:id="rId5" location="flightPageActivityLog" xr:uid="{0D1432A5-D70D-A641-98CE-1CDD0A717403}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>